<commit_message>
Added kolumn for present
Added possible dates for Anton to do labration
</commit_message>
<xml_diff>
--- a/Projectplan 240904.xlsx
+++ b/Projectplan 240904.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9595760148113650/Privat/Arduino/TrackRobot_AFS (Inbyggda System)/TrackBot_AFS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A835F0A3-805A-4FCE-A827-4F42E502F96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{A835F0A3-805A-4FCE-A827-4F42E502F96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53D5D352-EFD1-4B33-A4E0-EC008E38A116}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{1B8E7019-39E5-49FA-A016-6CE33A1C349C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="39">
   <si>
     <t>Date</t>
   </si>
@@ -147,13 +147,19 @@
   </si>
   <si>
     <t>Hand in laboration code</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Kanske</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -525,23 +531,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB012A7A-205F-4257-A52B-D06CE36627F5}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="5.6328125" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="6" max="6" width="6.25" customWidth="1"/>
+    <col min="7" max="7" width="6.58203125" customWidth="1"/>
+    <col min="8" max="8" width="4.83203125" customWidth="1"/>
+    <col min="9" max="9" width="12.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,10 +568,19 @@
         <v>20</v>
       </c>
       <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>45537</v>
       </c>
@@ -572,7 +591,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>45538</v>
       </c>
@@ -589,10 +608,19 @@
         <v>27</v>
       </c>
       <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>45539</v>
       </c>
@@ -606,7 +634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>45540</v>
       </c>
@@ -620,7 +648,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>45541</v>
       </c>
@@ -634,7 +662,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>45542</v>
       </c>
@@ -648,7 +676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>45543</v>
       </c>
@@ -662,7 +690,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>45544</v>
       </c>
@@ -675,8 +703,11 @@
       <c r="D9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>45545</v>
       </c>
@@ -693,10 +724,13 @@
         <v>27</v>
       </c>
       <c r="F10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>45546</v>
       </c>
@@ -712,8 +746,11 @@
       <c r="E11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>45547</v>
       </c>
@@ -727,7 +764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>45548</v>
       </c>
@@ -741,7 +778,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>45549</v>
       </c>
@@ -755,7 +792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>45550</v>
       </c>
@@ -769,7 +806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>45551</v>
       </c>
@@ -785,8 +822,14 @@
       <c r="E16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>45552</v>
       </c>
@@ -799,8 +842,11 @@
       <c r="D17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>45553</v>
       </c>
@@ -814,7 +860,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>45554</v>
       </c>
@@ -828,7 +874,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>45555</v>
       </c>
@@ -842,7 +888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>45556</v>
       </c>
@@ -856,7 +902,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>45557</v>
       </c>
@@ -870,7 +916,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>45558</v>
       </c>
@@ -884,7 +930,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>45559</v>
       </c>
@@ -898,7 +944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>45560</v>
       </c>
@@ -915,10 +961,13 @@
         <v>27</v>
       </c>
       <c r="F25" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>45561</v>
       </c>
@@ -932,7 +981,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>45562</v>
       </c>
@@ -946,7 +995,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>45563</v>
       </c>
@@ -960,7 +1009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>45564</v>
       </c>
@@ -974,7 +1023,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>45565</v>
       </c>
@@ -991,10 +1040,13 @@
         <v>27</v>
       </c>
       <c r="F30" t="s">
+        <v>37</v>
+      </c>
+      <c r="I30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>45566</v>
       </c>
@@ -1008,7 +1060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>45567</v>
       </c>
@@ -1022,7 +1074,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>45568</v>
       </c>
@@ -1036,7 +1088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>45569</v>
       </c>
@@ -1050,7 +1102,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>45570</v>
       </c>
@@ -1064,7 +1116,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>45571</v>
       </c>
@@ -1078,7 +1130,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>45572</v>
       </c>
@@ -1092,7 +1144,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>45573</v>
       </c>
@@ -1109,10 +1161,13 @@
         <v>27</v>
       </c>
       <c r="F38" t="s">
+        <v>37</v>
+      </c>
+      <c r="I38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>45574</v>
       </c>
@@ -1129,10 +1184,13 @@
         <v>27</v>
       </c>
       <c r="F39" t="s">
+        <v>38</v>
+      </c>
+      <c r="I39" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>45575</v>
       </c>
@@ -1146,7 +1204,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>45576</v>
       </c>
@@ -1160,7 +1218,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>45577</v>
       </c>
@@ -1174,7 +1232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>45578</v>
       </c>
@@ -1188,7 +1246,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>45579</v>
       </c>
@@ -1201,8 +1259,11 @@
       <c r="D44" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>45580</v>
       </c>
@@ -1219,10 +1280,13 @@
         <v>27</v>
       </c>
       <c r="F45" t="s">
+        <v>38</v>
+      </c>
+      <c r="I45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>45581</v>
       </c>
@@ -1236,7 +1300,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>45582</v>
       </c>
@@ -1250,7 +1314,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>45583</v>
       </c>
@@ -1264,7 +1328,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>45584</v>
       </c>
@@ -1278,7 +1342,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>45585</v>
       </c>
@@ -1292,7 +1356,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>45586</v>
       </c>
@@ -1305,8 +1369,11 @@
       <c r="D51" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>45587</v>
       </c>
@@ -1323,10 +1390,13 @@
         <v>27</v>
       </c>
       <c r="F52" t="s">
+        <v>37</v>
+      </c>
+      <c r="I52" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>45588</v>
       </c>
@@ -1343,10 +1413,13 @@
         <v>27</v>
       </c>
       <c r="F53" t="s">
+        <v>38</v>
+      </c>
+      <c r="I53" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>45589</v>
       </c>
@@ -1360,7 +1433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>45590</v>
       </c>
@@ -1374,7 +1447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>45591</v>
       </c>
@@ -1388,7 +1461,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>45592</v>
       </c>
@@ -1402,7 +1475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>45593</v>
       </c>
@@ -1416,7 +1489,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>45594</v>
       </c>
@@ -1432,8 +1505,11 @@
       <c r="E59" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F59" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>45595</v>
       </c>
@@ -1444,7 +1520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>45596</v>
       </c>
@@ -1455,7 +1531,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>45597</v>
       </c>
@@ -1466,7 +1542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>45598</v>
       </c>
@@ -1477,7 +1553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>45599</v>
       </c>
@@ -1488,7 +1564,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>45600</v>
       </c>
@@ -1499,7 +1575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>45601</v>
       </c>
@@ -1509,7 +1585,7 @@
       <c r="C66" t="s">
         <v>5</v>
       </c>
-      <c r="F66" t="s">
+      <c r="I66" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>